<commit_message>
added statistical analysis results
</commit_message>
<xml_diff>
--- a/HALVA-Statistical-Analysis.xlsx
+++ b/HALVA-Statistical-Analysis.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="70">
   <si>
     <t>Statistical analysis on general vision language tasks</t>
   </si>
@@ -23,7 +23,7 @@
     <t>We accept the performance drop in hallucination mitation method on general vision-language tasks is statistically significant if the adjusted_delta is greater than 0. We consider the standard error with statistical significance at 95% confidence.</t>
   </si>
   <si>
-    <t>original results are scaled between 0 to 1</t>
+    <t>original results are scaled between 0 to 1, where 0 represents the worst and 1 represents the best.</t>
   </si>
   <si>
     <t>TL;DR analysing if base_model is better than hallucination_mitigation_method on general tasks.</t>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>HADPO 7B worsen base model's performance in 2 out of 6 hallucination tasks.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MMHal-Bench </t>
   </si>
   <si>
     <t>EOS 7B worsen base model's performance in 2 out of 6 hallucination tasks and the performance drop on MME-Hall is statistically significant.</t>
@@ -31873,7 +31876,7 @@
     </row>
     <row r="58">
       <c r="A58" s="31" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B58" s="31">
         <v>0.46</v>
@@ -31952,7 +31955,7 @@
         <v>500.0</v>
       </c>
       <c r="H61" s="34" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="62">
@@ -32105,7 +32108,7 @@
         <v>500.0</v>
       </c>
       <c r="H68" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="69">
@@ -32258,7 +32261,7 @@
         <v>500.0</v>
       </c>
       <c r="H75" s="34" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76">
@@ -32411,7 +32414,7 @@
         <v>500.0</v>
       </c>
       <c r="H82" s="34" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83">

</xml_diff>